<commit_message>
Updated readme for sentiment and healthcare analysis
</commit_message>
<xml_diff>
--- a/Healthcare Dashboard - Excel/dashboard.xlsx
+++ b/Healthcare Dashboard - Excel/dashboard.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06c6126daff91742/Desktop/GIT_PROJECTS_DA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06c6126daff91742/Desktop/GIT_PROJECTS_DA/Healthcare Dashboard - Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7580E68C-FE1B-42E4-B042-A42EC6F61B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{7580E68C-FE1B-42E4-B042-A42EC6F61B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB576DDA-C676-495F-8AD4-AA67C707CF09}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{448A50DA-F215-4F3A-8D13-BFE628B692DE}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{876F7934-8845-4945-9796-88D515C7AA90}">
       <x14:pivotCaches>
-        <pivotCache cacheId="2" r:id="rId3"/>
+        <pivotCache cacheId="3" r:id="rId3"/>
       </x14:pivotCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -9869,8 +9869,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Cancer History 1">
@@ -9893,7 +9893,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -10051,8 +10051,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>50801</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="8" name="Weight Status 1">
@@ -10075,7 +10075,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -10129,8 +10129,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>110067</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="9" name="Diabetes Status 1">
@@ -10153,7 +10153,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -11306,8 +11306,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="12741341" y="5763824"/>
-            <a:ext cx="1100667" cy="465667"/>
+            <a:off x="13141801" y="5522016"/>
+            <a:ext cx="894000" cy="465667"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -11366,7 +11366,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="14395202" y="5733249"/>
-            <a:ext cx="1100667" cy="465667"/>
+            <a:ext cx="1100667" cy="325706"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -11573,8 +11573,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>533399</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>24553</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>340659</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11606,8 +11606,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4375573" y="33867"/>
-          <a:ext cx="364066" cy="364066"/>
+          <a:off x="4373780" y="33867"/>
+          <a:ext cx="364066" cy="306792"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -62119,7 +62119,7 @@
   <dimension ref="C1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>